<commit_message>
fix: improve error handling in file upload and update test data
</commit_message>
<xml_diff>
--- a/backend/test_data.xlsx
+++ b/backend/test_data.xlsx
@@ -1,10 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28623"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{4104EB3B-02D4-4E21-9391-114CD2DFBBE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet sheetId="1" name="Recipients" state="visible" r:id="rId4"/>
+    <sheet name="Recipients" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
@@ -52,9 +56,6 @@
     <t>Jane Smith</t>
   </si>
   <si>
-    <t>jane.smith@example.com</t>
-  </si>
-  <si>
     <t>Ms.</t>
   </si>
   <si>
@@ -62,22 +63,35 @@
   </si>
   <si>
     <t>Project Manager</t>
+  </si>
+  <si>
+    <t>insomewhererandom@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -97,14 +111,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -441,14 +458,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F3"/>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="6" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -468,7 +490,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -488,28 +510,31 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>12</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
         <v>13</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>14</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>15</v>
-      </c>
-      <c r="E3" t="s">
-        <v>16</v>
       </c>
       <c r="F3" t="s">
         <v>11</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{9A20D0A1-EFD0-414F-83CE-2A2FA3DF123E}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix: convert date values to strings in Excel parsing
</commit_message>
<xml_diff>
--- a/backend/test_data.xlsx
+++ b/backend/test_data.xlsx
@@ -1,14 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28623"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{4104EB3B-02D4-4E21-9391-114CD2DFBBE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-  </bookViews>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
-    <sheet name="Recipients" sheetId="1" r:id="rId1"/>
+    <sheet sheetId="1" name="Recipients" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
@@ -56,6 +52,9 @@
     <t>Jane Smith</t>
   </si>
   <si>
+    <t>jane.smith@example.com</t>
+  </si>
+  <si>
     <t>Ms.</t>
   </si>
   <si>
@@ -63,35 +62,22 @@
   </si>
   <si>
     <t>Project Manager</t>
-  </si>
-  <si>
-    <t>insomewhererandom@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <b/>
     </font>
   </fonts>
   <fills count="2">
@@ -111,17 +97,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -458,19 +441,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F3"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="6" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -490,7 +468,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -510,31 +488,28 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" t="s">
         <v>16</v>
-      </c>
-      <c r="C3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" t="s">
-        <v>15</v>
       </c>
       <c r="F3" t="s">
         <v>11</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" xr:uid="{9A20D0A1-EFD0-414F-83CE-2A2FA3DF123E}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>
 </file>
</xml_diff>